<commit_message>
addition of updated pete csv, continued analysis on cohort behavior
</commit_message>
<xml_diff>
--- a/notebooks/df5.xlsx
+++ b/notebooks/df5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erinm\Documents\donations\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2864CF64-8810-4EC3-8A62-3515EA6930DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E2C463-710D-4CB0-94A0-630A7B4E4E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df5 (2)" sheetId="3" r:id="rId1"/>
@@ -3131,7 +3131,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13933,15 +13933,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>86</xdr:col>
-      <xdr:colOff>384810</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>92</xdr:col>
-      <xdr:colOff>422910</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>93</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14144,59 +14144,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>87</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>88</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{844D9494-41CD-4959-BAA7-3C5796E28D35}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7551420" y="5615940"/>
-          <a:ext cx="659130" cy="788670"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -14784,6 +14731,54 @@
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="2707005" y="432436"/>
           <a:ext cx="605790" cy="140970"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.27944</cdr:x>
+      <cdr:y>0.53503</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.4161</cdr:x>
+      <cdr:y>0.66632</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD8AF953-2E64-4FFA-A430-957EBB33FA86}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1277620" y="1925320"/>
+          <a:ext cx="624810" cy="472453"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
           <a:avLst/>
@@ -15421,7 +15416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F3346B-BCAB-404C-8846-0900C7E49A28}">
   <dimension ref="A1:CU113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
@@ -39827,7 +39822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="CP105" sqref="CP105"/>
     </sheetView>
   </sheetViews>
@@ -64234,7 +64229,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
       <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>

</xml_diff>